<commit_message>
absent, is half day, document, print leave
</commit_message>
<xml_diff>
--- a/WebTemplate/Resources/Template/Medicard.xlsx
+++ b/WebTemplate/Resources/Template/Medicard.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIS 3\source\repos\TPJ-HRIS\WebTemplate\Resources\Template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600"/>
   </bookViews>
@@ -11,6 +16,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$AA$26</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -93,8 +101,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,16 +292,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -335,56 +343,56 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -392,6 +400,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -438,7 +454,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -470,9 +486,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -504,6 +521,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -679,14 +697,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="X24" sqref="X24:Z24"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:Z22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
     <col min="2" max="2" width="4.5703125" style="2" customWidth="1"/>
@@ -717,38 +735,38 @@
     <col min="28" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="27" customHeight="1">
+    <row r="1" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25"/>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
       <c r="AA1" s="9"/>
     </row>
-    <row r="2" spans="1:27" ht="8.25" customHeight="1">
+    <row r="2" spans="1:27" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>21</v>
       </c>
@@ -779,7 +797,7 @@
       <c r="Z2" s="3"/>
       <c r="AA2" s="11"/>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="18" t="s">
         <v>0</v>
@@ -789,13 +807,13 @@
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -805,14 +823,14 @@
         <v>2</v>
       </c>
       <c r="U3" s="5"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="35"/>
-      <c r="Y3" s="35"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="6" t="s">
         <v>1</v>
@@ -820,13 +838,13 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -839,13 +857,13 @@
       </c>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="36"/>
+      <c r="W4" s="33"/>
+      <c r="X4" s="33"/>
+      <c r="Y4" s="33"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="11"/>
     </row>
-    <row r="5" spans="1:27" ht="12.75" customHeight="1">
+    <row r="5" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -874,19 +892,19 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="11"/>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
       <c r="M6" s="21"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -896,15 +914,15 @@
         <v>5</v>
       </c>
       <c r="T6" s="4"/>
-      <c r="U6" s="36"/>
-      <c r="V6" s="36"/>
-      <c r="W6" s="36"/>
-      <c r="X6" s="36"/>
-      <c r="Y6" s="36"/>
+      <c r="U6" s="33"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="33"/>
+      <c r="X6" s="33"/>
+      <c r="Y6" s="33"/>
       <c r="Z6" s="4"/>
       <c r="AA6" s="11"/>
     </row>
-    <row r="7" spans="1:27" ht="7.5" customHeight="1">
+    <row r="7" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -933,95 +951,95 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="11"/>
     </row>
-    <row r="8" spans="1:27" ht="8.25" customHeight="1" thickBot="1">
+    <row r="8" spans="1:27" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="27" t="s">
+      <c r="M8" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="27" t="s">
+      <c r="V8" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="W8" s="27"/>
-      <c r="X8" s="27"/>
+      <c r="W8" s="26"/>
+      <c r="X8" s="26"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="11"/>
     </row>
-    <row r="9" spans="1:27" ht="6" customHeight="1" thickBot="1">
+    <row r="9" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
-      <c r="U9" s="22"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="27"/>
-      <c r="X9" s="27"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="26"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="11"/>
     </row>
-    <row r="10" spans="1:27" ht="6" customHeight="1">
+    <row r="10" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="V10" s="27"/>
-      <c r="W10" s="27"/>
-      <c r="X10" s="27"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+      <c r="V10" s="26"/>
+      <c r="W10" s="26"/>
+      <c r="X10" s="26"/>
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
       <c r="AA10" s="13"/>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
@@ -1031,19 +1049,19 @@
       <c r="E11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5" t="s">
         <v>2</v>
       </c>
       <c r="M11" s="5"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
@@ -1052,77 +1070,77 @@
         <v>2</v>
       </c>
       <c r="V11" s="5"/>
-      <c r="W11" s="35"/>
-      <c r="X11" s="35"/>
+      <c r="W11" s="32"/>
+      <c r="X11" s="32"/>
       <c r="Y11" s="5"/>
       <c r="Z11" s="5"/>
       <c r="AA11" s="14"/>
     </row>
-    <row r="12" spans="1:27" ht="8.25" customHeight="1" thickBot="1">
+    <row r="12" spans="1:27" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="29" t="s">
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="29"/>
+      <c r="J12" s="28"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="28" t="s">
+      <c r="M12" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
-      <c r="U12" s="28" t="s">
+      <c r="U12" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="V12" s="28"/>
-      <c r="W12" s="37"/>
-      <c r="X12" s="37"/>
+      <c r="V12" s="27"/>
+      <c r="W12" s="36"/>
+      <c r="X12" s="36"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="11"/>
     </row>
-    <row r="13" spans="1:27" ht="6" customHeight="1" thickBot="1">
+    <row r="13" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
-      <c r="U13" s="28"/>
-      <c r="V13" s="28"/>
-      <c r="W13" s="38"/>
-      <c r="X13" s="38"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="37"/>
+      <c r="X13" s="37"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="11"/>
     </row>
-    <row r="14" spans="1:27" ht="6" customHeight="1">
+    <row r="14" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1131,43 +1149,43 @@
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="U14" s="28"/>
-      <c r="V14" s="28"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="U14" s="27"/>
+      <c r="V14" s="27"/>
       <c r="W14" s="20"/>
       <c r="X14" s="20"/>
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
       <c r="AA14" s="13"/>
     </row>
-    <row r="15" spans="1:27" ht="4.5" customHeight="1" thickBot="1">
+    <row r="15" spans="1:27" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="32" t="s">
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="32"/>
+      <c r="J15" s="31"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="28" t="s">
+      <c r="M15" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="N15" s="28"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -1180,23 +1198,23 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="11"/>
     </row>
-    <row r="16" spans="1:27" ht="6" customHeight="1" thickBot="1">
+    <row r="16" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -1209,7 +1227,7 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="11"/>
     </row>
-    <row r="17" spans="1:27" ht="3.75" customHeight="1">
+    <row r="17" spans="1:27" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1218,14 +1236,14 @@
       <c r="F17" s="20"/>
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
       <c r="U17" s="1"/>
       <c r="V17" s="20"/>
       <c r="W17" s="20"/>
@@ -1234,7 +1252,7 @@
       <c r="Z17" s="7"/>
       <c r="AA17" s="13"/>
     </row>
-    <row r="18" spans="1:27" ht="27" customHeight="1">
+    <row r="18" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1243,14 +1261,14 @@
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
       <c r="U18" s="1"/>
       <c r="V18" s="20"/>
       <c r="W18" s="20"/>
@@ -1259,127 +1277,127 @@
       <c r="Z18" s="7"/>
       <c r="AA18" s="13"/>
     </row>
-    <row r="19" spans="1:27" ht="15" customHeight="1">
+    <row r="19" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="35"/>
-      <c r="S19" s="35"/>
-      <c r="T19" s="35"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="35"/>
-      <c r="X19" s="35"/>
-      <c r="Y19" s="35"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="32"/>
+      <c r="W19" s="32"/>
+      <c r="X19" s="32"/>
+      <c r="Y19" s="32"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="11"/>
     </row>
-    <row r="20" spans="1:27">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="6"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="36"/>
-      <c r="X20" s="36"/>
-      <c r="Y20" s="36"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="33"/>
+      <c r="S20" s="33"/>
+      <c r="T20" s="33"/>
+      <c r="U20" s="33"/>
+      <c r="V20" s="33"/>
+      <c r="W20" s="33"/>
+      <c r="X20" s="33"/>
+      <c r="Y20" s="33"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="11"/>
     </row>
-    <row r="21" spans="1:27" ht="21.75" customHeight="1">
+    <row r="21" spans="1:27" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="26"/>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="26"/>
-      <c r="W21" s="26"/>
-      <c r="X21" s="26"/>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="26"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
+      <c r="S21" s="25"/>
+      <c r="T21" s="25"/>
+      <c r="U21" s="25"/>
+      <c r="V21" s="25"/>
+      <c r="W21" s="25"/>
+      <c r="X21" s="25"/>
+      <c r="Y21" s="25"/>
+      <c r="Z21" s="25"/>
       <c r="AA21" s="11"/>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="26"/>
-      <c r="W22" s="26"/>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="26"/>
-      <c r="Z22" s="26"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="25"/>
+      <c r="S22" s="25"/>
+      <c r="T22" s="25"/>
+      <c r="U22" s="25"/>
+      <c r="V22" s="25"/>
+      <c r="W22" s="25"/>
+      <c r="X22" s="25"/>
+      <c r="Y22" s="25"/>
+      <c r="Z22" s="25"/>
       <c r="AA22" s="11"/>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="6" t="s">
         <v>14</v>
@@ -1413,36 +1431,36 @@
       <c r="Z23" s="6"/>
       <c r="AA23" s="11"/>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="35"/>
-      <c r="P24" s="35"/>
-      <c r="Q24" s="35"/>
-      <c r="R24" s="35"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="32"/>
+      <c r="R24" s="32"/>
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
-      <c r="X24" s="35"/>
-      <c r="Y24" s="35"/>
-      <c r="Z24" s="35"/>
+      <c r="X24" s="32"/>
+      <c r="Y24" s="32"/>
+      <c r="Z24" s="32"/>
       <c r="AA24" s="11"/>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="19" t="s">
         <v>19</v>
@@ -1455,29 +1473,29 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="33" t="s">
+      <c r="K25" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-      <c r="N25" s="33"/>
-      <c r="O25" s="33"/>
-      <c r="P25" s="33"/>
-      <c r="Q25" s="33"/>
-      <c r="R25" s="33"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
+      <c r="P25" s="34"/>
+      <c r="Q25" s="34"/>
+      <c r="R25" s="34"/>
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
-      <c r="X25" s="33" t="s">
+      <c r="X25" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Y25" s="33"/>
-      <c r="Z25" s="33"/>
+      <c r="Y25" s="34"/>
+      <c r="Z25" s="34"/>
       <c r="AA25" s="11"/>
     </row>
-    <row r="26" spans="1:27" ht="6" customHeight="1">
+    <row r="26" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -1538,30 +1556,30 @@
     <mergeCell ref="G6:L6"/>
     <mergeCell ref="U6:Y6"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>